<commit_message>
add 2.1.2: add chieukhau theo sl
</commit_message>
<xml_diff>
--- a/ReadAndWriteFileExcel/TrungTrang/bin/Debug/excel/phieusuachua.xlsx
+++ b/ReadAndWriteFileExcel/TrungTrang/bin/Debug/excel/phieusuachua.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\exceltrungtrang\ReadAndWriteFileExcel\TrungTrang\bin\Debug\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBAEEAD-5DB1-4BD3-9187-0621060D87BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A0FD94-527B-4EDF-902A-3E3DEFE4AC31}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11655" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2553,8 +2553,8 @@
   </sheetPr>
   <dimension ref="A1:IV60"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AJ44" sqref="AJ44:AK44"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="B20" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AG45" sqref="AG45:AI45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15"/>
@@ -3609,7 +3609,7 @@
       <c r="W25" s="187"/>
       <c r="X25" s="187"/>
       <c r="Y25" s="184">
-        <f>ROUND(V25*O25,-1)</f>
+        <f>ROUND(V25*AC25,-1)</f>
         <v>0</v>
       </c>
       <c r="Z25" s="184"/>
@@ -3628,7 +3628,7 @@
       <c r="AH25" s="171"/>
       <c r="AI25" s="171"/>
       <c r="AJ25" s="171">
-        <f>AC25-Y25*T25 + ROUND(AG25*(1-V25),-1)</f>
+        <f>AC25-Y25 + ROUND(AG25*(1-V25),-1)</f>
         <v>0</v>
       </c>
       <c r="AK25" s="172"/>
@@ -3668,7 +3668,7 @@
       <c r="W26" s="187"/>
       <c r="X26" s="187"/>
       <c r="Y26" s="184">
-        <f t="shared" ref="Y26:Y44" si="0">ROUND(V26*O26,-1)</f>
+        <f t="shared" ref="Y26:Y44" si="0">ROUND(V26*AC26,-1)</f>
         <v>0</v>
       </c>
       <c r="Z26" s="184"/>
@@ -3687,7 +3687,7 @@
       <c r="AH26" s="210"/>
       <c r="AI26" s="211"/>
       <c r="AJ26" s="171">
-        <f t="shared" ref="AJ26:AJ44" si="2">AC26-Y26*T26 + ROUND(AG26*(1-V26),-1)</f>
+        <f t="shared" ref="AJ26:AJ44" si="2">AC26-Y26 + ROUND(AG26*(1-V26),-1)</f>
         <v>0</v>
       </c>
       <c r="AK26" s="172"/>
@@ -5103,7 +5103,7 @@
       <c r="AA45" s="207"/>
       <c r="AB45" s="207"/>
       <c r="AC45" s="206">
-        <f>SUMPRODUCT( (AC25:AF44)  - (Y25:AB44)* (T25:T44))</f>
+        <f>SUMPRODUCT( (AC25:AF44)  - (Y25:AB44))</f>
         <v>0</v>
       </c>
       <c r="AD45" s="206"/>

</xml_diff>